<commit_message>
plots recollected to add in thesis
</commit_message>
<xml_diff>
--- a/trials_waiwera/onur2008/one_cell_1e7_vol_onur2008/onur_calc.xlsx
+++ b/trials_waiwera/onur2008/one_cell_1e7_vol_onur2008/onur_calc.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myvuwac-my.sharepoint.com/personal/duggalrohi_myvuw_ac_nz/Documents/wai_sim/simulation/trials/onur2008/one_cell_1e7_vol_onur2008/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myvuwac-my.sharepoint.com/personal/duggalrohi_myvuw_ac_nz/Documents/wai_sim/simulation/trials_waiwera/onur2008/one_cell_1e7_vol_onur2008/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="734" documentId="8_{039A52CA-99B0-4142-ABD1-75F49B448DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B7049AA-E61A-4512-B2AB-0A7AB39479A6}"/>
+  <xr:revisionPtr revIDLastSave="767" documentId="8_{039A52CA-99B0-4142-ABD1-75F49B448DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59ACEE30-8911-4127-81D5-B4C9154CD108}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{E8903688-4988-4AD0-AA47-6FBF2596F01C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{E8903688-4988-4AD0-AA47-6FBF2596F01C}"/>
   </bookViews>
   <sheets>
     <sheet name="onurT" sheetId="6" r:id="rId1"/>
     <sheet name="one_cell_1e7_vol_onur2008" sheetId="1" r:id="rId2"/>
-    <sheet name="one_cell_1m3_vol" sheetId="8" r:id="rId3"/>
-    <sheet name="one_cell_25e9_vol" sheetId="7" r:id="rId4"/>
-    <sheet name="sat_water" sheetId="4" r:id="rId5"/>
-    <sheet name="Sheet0" sheetId="5" r:id="rId6"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId7"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId3"/>
+    <sheet name="one_cell_1m3_vol" sheetId="8" r:id="rId4"/>
+    <sheet name="one_cell_25e9_vol" sheetId="7" r:id="rId5"/>
+    <sheet name="sat_water" sheetId="4" r:id="rId6"/>
+    <sheet name="Sheet0" sheetId="5" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId8"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -989,11 +990,17 @@
     <numFmt numFmtId="165" formatCode="0.00000000000000000000000000000"/>
     <numFmt numFmtId="166" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -1089,8 +1096,8 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1099,10 +1106,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1802,7 +1809,454 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$12:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$12:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>47.577736848379502</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45.155473696758996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42.733210545138505</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.311733553195701</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37.893920005406599</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35.4763249490818</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.058729892756901</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30.641134836432101</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28.223539780107203</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25.8059447237824</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>23.388349667457501</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20.977329892021199</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18.5678693434187</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16.1584087948162</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.7489482462138</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11.3394876976113</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.9300271490088008</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.5205666004063003</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.1176050327351001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.7162274991658999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-61CB-465F-80AA-BF7FB96696F8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1336441055"/>
+        <c:axId val="1336441471"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1336441055"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1336441471"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1336441471"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1336441055"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2358,20 +2812,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>647701</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>795113</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>163739</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>352426</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>465820</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>181429</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2379,6 +3349,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE348414-36D4-41D7-9F47-77CB58D31135}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A2BDE70-4AE7-96DE-D95E-A6EB7EEEECD0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4409,8 +5420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD6DAF24-5525-4D03-BF9A-8F00D4E1F5A6}">
   <dimension ref="A1:AG73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G21" zoomScale="84" workbookViewId="0">
-      <selection activeCell="AH56" sqref="AH56"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="AB29" sqref="AB29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4724,7 +5735,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="16" spans="1:33" ht="20.25" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="N16" t="s">
         <v>241</v>
       </c>
@@ -4955,7 +5966,7 @@
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="N19" s="3">
-        <f t="shared" ref="N18:N32" si="6">P19-((Q19*R19)/(V19))</f>
+        <f t="shared" ref="N19:N32" si="6">P19-((Q19*R19)/(V19))</f>
         <v>4978135.9699733984</v>
       </c>
       <c r="O19" s="13">
@@ -4985,7 +5996,7 @@
         <v>2.0244472246853</v>
       </c>
       <c r="V19" s="5">
-        <f t="shared" ref="V18:V32" si="8">W19*X19*Y19*Z19</f>
+        <f t="shared" ref="V19:V32" si="8">W19*X19*Y19*Z19</f>
         <v>2.4698099999999998</v>
       </c>
       <c r="W19" s="5">
@@ -6302,7 +7313,7 @@
     <row r="52" spans="14:31" x14ac:dyDescent="0.25">
       <c r="AB52" s="5"/>
     </row>
-    <row r="53" spans="14:31" ht="20.25" x14ac:dyDescent="0.5">
+    <row r="53" spans="14:31" x14ac:dyDescent="0.25">
       <c r="N53" t="s">
         <v>241</v>
       </c>
@@ -6566,7 +7577,7 @@
         <v>4.0054433975964478E-5</v>
       </c>
       <c r="AE57">
-        <f t="shared" ref="AE55:AE57" si="18">AD57/100000</f>
+        <f t="shared" ref="AE57" si="18">AD57/100000</f>
         <v>4.0054433975964478E-10</v>
       </c>
     </row>
@@ -7320,11 +8331,417 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09BBFCED-5056-4C74-8D49-4B03E0DAAAFA}">
+  <dimension ref="B4:I31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>4757773.6848379504</v>
+      </c>
+      <c r="F4">
+        <v>4515547.3696758999</v>
+      </c>
+      <c r="G4">
+        <v>4273321.0545138502</v>
+      </c>
+      <c r="H4">
+        <v>4031173.3553195698</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>3789392.0005406602</v>
+      </c>
+      <c r="G5">
+        <v>3547632.4949081801</v>
+      </c>
+      <c r="H5">
+        <v>3305872.9892756902</v>
+      </c>
+      <c r="I5">
+        <v>3064113.48364321</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>2822353.9780107201</v>
+      </c>
+      <c r="G6">
+        <v>2580594.47237824</v>
+      </c>
+      <c r="H6">
+        <v>2338834.96674575</v>
+      </c>
+      <c r="I6">
+        <v>2097732.9892021199</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>1856786.93434187</v>
+      </c>
+      <c r="G7">
+        <v>1615840.8794816199</v>
+      </c>
+      <c r="H7">
+        <v>1374894.8246213801</v>
+      </c>
+      <c r="I7">
+        <v>1133948.76976113</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>893002.71490088</v>
+      </c>
+      <c r="G8">
+        <v>652056.66004063003</v>
+      </c>
+      <c r="H8">
+        <v>411760.50327351002</v>
+      </c>
+      <c r="I8">
+        <v>171622.74991658999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>43200</v>
+      </c>
+      <c r="C12">
+        <f>B12/(3600*24)</f>
+        <v>0.5</v>
+      </c>
+      <c r="D12">
+        <f>E12/100000</f>
+        <v>47.577736848379502</v>
+      </c>
+      <c r="E12">
+        <v>4757773.6848379504</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>86400</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:C31" si="0">B13/(3600*24)</f>
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:D31" si="1">E13/100000</f>
+        <v>45.155473696758996</v>
+      </c>
+      <c r="E13">
+        <v>4515547.3696758999</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>129600</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>42.733210545138505</v>
+      </c>
+      <c r="E14">
+        <v>4273321.0545138502</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>172800</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>40.311733553195701</v>
+      </c>
+      <c r="E15">
+        <v>4031173.3553195698</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>216000</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>37.893920005406599</v>
+      </c>
+      <c r="E16">
+        <v>3789392.0005406602</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>259200</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>35.4763249490818</v>
+      </c>
+      <c r="E17">
+        <v>3547632.4949081801</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>302400</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>33.058729892756901</v>
+      </c>
+      <c r="E18">
+        <v>3305872.9892756902</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>345600</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>30.641134836432101</v>
+      </c>
+      <c r="E19">
+        <v>3064113.48364321</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>388800</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>28.223539780107203</v>
+      </c>
+      <c r="E20">
+        <v>2822353.9780107201</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>432000</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>25.8059447237824</v>
+      </c>
+      <c r="E21">
+        <v>2580594.47237824</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>475200</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>23.388349667457501</v>
+      </c>
+      <c r="E22">
+        <v>2338834.96674575</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>518400</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>20.977329892021199</v>
+      </c>
+      <c r="E23">
+        <v>2097732.9892021199</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>561600</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>18.5678693434187</v>
+      </c>
+      <c r="E24">
+        <v>1856786.93434187</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>604800</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>16.1584087948162</v>
+      </c>
+      <c r="E25">
+        <v>1615840.8794816199</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>648000</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>13.7489482462138</v>
+      </c>
+      <c r="E26">
+        <v>1374894.8246213801</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>691200</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>11.3394876976113</v>
+      </c>
+      <c r="E27">
+        <v>1133948.76976113</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>734400</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>8.9300271490088008</v>
+      </c>
+      <c r="E28">
+        <v>893002.71490088</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>777600</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>6.5205666004063003</v>
+      </c>
+      <c r="E29">
+        <v>652056.66004063003</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>820800</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>4.1176050327351001</v>
+      </c>
+      <c r="E30">
+        <v>411760.50327351002</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>864000</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>1.7162274991658999</v>
+      </c>
+      <c r="E31">
+        <v>171622.74991658999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C48BD2F-6946-4853-9EA3-929E5FD417E8}">
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A3" sqref="A3:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7339,7 +8756,7 @@
       </c>
       <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:18" ht="20.25" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>241</v>
       </c>
@@ -8350,7 +9767,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22CE7212-342D-4586-8EE5-1239AB6CEB54}">
   <dimension ref="A1:M18"/>
   <sheetViews>
@@ -8366,7 +9783,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="20.25" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>241</v>
       </c>
@@ -9164,7 +10581,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDDFEAE-E430-41B9-A665-61CE6C1D4DF0}">
   <dimension ref="A1:P58"/>
   <sheetViews>
@@ -12097,13 +13514,13 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD7A80C-4E81-44EF-8FB6-146C1A4C34D8}">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -12231,7 +13648,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89BAAEB5-97C8-4429-8196-CB6BF4254EFB}">
   <dimension ref="A1:H63"/>
   <sheetViews>
@@ -13361,7 +14778,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784E863C-D2B1-4672-93BF-1E7092688CE1}">
   <dimension ref="A1:A39"/>
   <sheetViews>

</xml_diff>